<commit_message>
Files added, code compiled, bugs and issues resolved
</commit_message>
<xml_diff>
--- a/DATABASE.xlsx
+++ b/DATABASE.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,6 +555,53 @@
       <c r="I3" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>asdfl;k</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>saflk;j</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>salkfjlk</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>slkfaj</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>lksfdajlk</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>lkdsafj</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added feature for emplyee attendance
</commit_message>
<xml_diff>
--- a/DATABASE.xlsx
+++ b/DATABASE.xlsx
@@ -4,12 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="EMP_RECORD" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="BACKUP_EMP_RECORD" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="EMP_ATTENDANCE" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,177 +432,257 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Chetan</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Chinchulakr</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sldakfj</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fasldkfj</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>flsdkjafls</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mornnig</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Chetan</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Chinchulkar</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>EP</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Junior</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Stud</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Chinchulakr</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>sldakfj</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>fasldkfj</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>flsdkjafls</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>mornnig</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>Chetan</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Chinchulkar</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>EP</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Junior</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Stud</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Chinchulakrsdafds</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>sldakfj</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fasldkfj</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>flsdkjafls</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>mornnig</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Chetands</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Chinchulkar</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>EP</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Junior</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Stud</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Chetanss</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Chinchulakrsdafds</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>sldakfj</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>fasldkfj</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>flsdkjafls</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>mornnig</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>asdfl;k</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>saflk;j</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>salkfjlk</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>slkfaj</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>lksfdajlk</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>lkdsafj</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>33</t>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>232</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Che222</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Chinchulakrsdafds</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>sldakfj</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>fasldkfj</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>flsdkjafls</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>mornnig</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Che222</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Chinchrsdafds</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>sldakfj</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>fasldkfj</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>flsdkjafls</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>mornnig</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -634,6 +715,127 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>EMP_ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>TIME</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>29-06-2022</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>17:20:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>29-06-2022</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>17:21:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>29-06-2022</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>17:22:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>29-06-2022</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>17:23:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>29-06-2022</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>17:23:20</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
highlight added for empty ID
</commit_message>
<xml_diff>
--- a/DATABASE.xlsx
+++ b/DATABASE.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="EMP_RECORD" sheetId="1" state="visible" r:id="rId1"/>
@@ -416,277 +416,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Chetan</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Chinchulakr</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sldakfj</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>fasldkfj</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>flsdkjafls</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>mornnig</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Chetan</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Chinchulakr</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>sldakfj</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>fasldkfj</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>flsdkjafls</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>mornnig</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Chetan</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Chinchulakrsdafds</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>sldakfj</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>fasldkfj</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>flsdkjafls</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>mornnig</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Chetanss</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Chinchulakrsdafds</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>sldakfj</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>fasldkfj</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>flsdkjafls</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>mornnig</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>232</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Che222</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Chinchulakrsdafds</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>sldakfj</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>fasldkfj</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>flsdkjafls</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>mornnig</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Che222</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Chinchrsdafds</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>sldakfj</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>fasldkfj</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>flsdkjafls</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>mornnig</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -715,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -753,75 +490,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>17:20:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>29-06-2022</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>17:21:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>29-06-2022</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>17:22:03</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>29-06-2022</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>17:23:08</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>29-06-2022</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>17:23:20</t>
+          <t>17:34:40</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to have common splash screen for login
</commit_message>
<xml_diff>
--- a/DATABASE.xlsx
+++ b/DATABASE.xlsx
@@ -416,14 +416,156 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Chetan</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Chinchulkar</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>safdsf</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>fsadf</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dfdsa</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Chetan</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Chinchulkar</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>safdsf</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>fsadf</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>dfdsa</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>323</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chetansdafdsf</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Chinchulkar</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>safdsf</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>fsadf</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>dfdsa</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -452,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +633,40 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>17:34:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>03-07-2022</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>21:27:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>323</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>03-07-2022</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>21:28:04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
NEILIT logo changed to GPlus
</commit_message>
<xml_diff>
--- a/DATABASE.xlsx
+++ b/DATABASE.xlsx
@@ -594,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,6 +684,23 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>19:47:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>05-07-2022</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20:13:08</t>
         </is>
       </c>
     </row>

</xml_diff>